<commit_message>
Change yoda importing to fix issue with lab information.
</commit_message>
<xml_diff>
--- a/storage/app/import-data/yoda/Datapublicaties_EPOS_v07.xlsx
+++ b/storage/app/import-data/yoda/Datapublicaties_EPOS_v07.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/v_brunst_uu_nl/Documents/Own Documents/EPOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samsh001\Projects\epos\storage\app\import-data\yoda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="8_{D3B4EB91-EA80-4792-98CB-D316C4228758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B68F2A03-4F5B-43C5-B6F1-39313A86D03A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E4ECCE-643A-45D4-889E-847BBA38E833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A489FE1-54A2-4982-833C-473B31F78788}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A489FE1-54A2-4982-833C-473B31F78788}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -389,12 +389,6 @@
     <t>https://geo.public.data.uu.nl/vault-groningen-zandsteencompactie/research-groningen-zandsteencompactie%5B1667459035%5D/original/Additional_explanation_to_the_data.pdf</t>
   </si>
   <si>
-    <t>Laboratory</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
     <t>aa45f98e5c098237d0c57b58e5f953e1</t>
   </si>
   <si>
@@ -522,6 +516,12 @@
   </si>
   <si>
     <t>https://geo.public.data.uu.nl/vault-alteredbasaltfriction/research-alteredbasaltfriction%5B1671698883%5D/original/Okuda-et-al-2022-Data-Description.pdf</t>
+  </si>
+  <si>
+    <t>LabName</t>
+  </si>
+  <si>
+    <t>LabIdentifier</t>
   </si>
 </sst>
 </file>
@@ -899,22 +899,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F10554-A53B-41FD-AC2A-9DF004AA7FB9}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="74.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="79.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="74.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="79.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="77" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -940,13 +940,13 @@
         <v>81</v>
       </c>
       <c r="I1" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="J1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -969,13 +969,13 @@
         <v>83</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -999,13 +999,13 @@
         <v>84</v>
       </c>
       <c r="I3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+1</f>
         <v>3</v>
@@ -1029,13 +1029,13 @@
         <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+1</f>
         <v>4</v>
@@ -1059,13 +1059,13 @@
         <v>86</v>
       </c>
       <c r="I5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5+1</f>
         <v>5</v>
@@ -1089,13 +1089,13 @@
         <v>87</v>
       </c>
       <c r="I6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6+1</f>
         <v>6</v>
@@ -1119,10 +1119,10 @@
         <v>88</v>
       </c>
       <c r="J7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ref="A8:A22" si="0">A7+1</f>
         <v>7</v>
@@ -1146,13 +1146,13 @@
         <v>89</v>
       </c>
       <c r="I8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1176,13 +1176,13 @@
         <v>90</v>
       </c>
       <c r="I9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1206,13 +1206,13 @@
         <v>91</v>
       </c>
       <c r="I10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1236,13 +1236,13 @@
         <v>92</v>
       </c>
       <c r="I11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1266,13 +1266,13 @@
         <v>93</v>
       </c>
       <c r="I12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1296,13 +1296,13 @@
         <v>94</v>
       </c>
       <c r="I13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1326,13 +1326,13 @@
         <v>95</v>
       </c>
       <c r="I14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1356,13 +1356,13 @@
         <v>96</v>
       </c>
       <c r="I15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1386,13 +1386,13 @@
         <v>97</v>
       </c>
       <c r="I16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1416,13 +1416,13 @@
         <v>98</v>
       </c>
       <c r="I17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1446,13 +1446,13 @@
         <v>99</v>
       </c>
       <c r="I18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J18" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1476,13 +1476,13 @@
         <v>100</v>
       </c>
       <c r="I19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1503,13 +1503,13 @@
         <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1533,13 +1533,13 @@
         <v>101</v>
       </c>
       <c r="I21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J21" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1563,13 +1563,13 @@
         <v>102</v>
       </c>
       <c r="I22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1592,13 +1592,13 @@
         <v>103</v>
       </c>
       <c r="I23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1621,13 +1621,13 @@
         <v>104</v>
       </c>
       <c r="I24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J24" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1650,13 +1650,13 @@
         <v>112</v>
       </c>
       <c r="I25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1682,13 +1682,13 @@
         <v>109</v>
       </c>
       <c r="I26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1714,24 +1714,24 @@
         <v>116</v>
       </c>
       <c r="I27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="E28" t="s">
         <v>80</v>
@@ -1740,174 +1740,174 @@
         <v>5</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F30" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="H31" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F31" t="s">
-        <v>16</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="H32" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="F32" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F33" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>153</v>
-      </c>
       <c r="I33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J33" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="H34" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="F34" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="D35" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="E35" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>